<commit_message>
Update package to xyz;Fixed the bug for convert the date content
</commit_message>
<xml_diff>
--- a/src/test/resources/normalWithTitle.xlsx
+++ b/src/test/resources/normalWithTitle.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiang/workspace/private/ProteanBear/PbPOITemplate/src/test/java/com/github/ProteanBear/template/excel/file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiang/workspace/private/ProteanBear/PbPOITemplate/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEFFB57-8D5F-CB44-BCF6-249D286D497D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -81,10 +82,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="181" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -144,19 +145,19 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -169,6 +170,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -436,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix Bug：When numeric field content is blank,Parsing throw a exception
</commit_message>
<xml_diff>
--- a/src/test/resources/normalWithTitle.xlsx
+++ b/src/test/resources/normalWithTitle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiang/workspace/private/ProteanBear/PbPOITemplate/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiang/编程/poi-template/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C9F93C-E3ED-7543-AEBF-3D1ACA0119FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9915AB-79E3-784F-AF4E-1053C005C0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>标题</t>
     <rPh sb="0" eb="1">
@@ -69,6 +69,10 @@
     <rPh sb="0" eb="1">
       <t>ni'hao</t>
     </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -434,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,6 +499,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>